<commit_message>
feat: More training completed
</commit_message>
<xml_diff>
--- a/project-3/agile-communication-exercises-template-9320.xlsx
+++ b/project-3/agile-communication-exercises-template-9320.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="606" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="1. Scrum Exercise" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,236 +20,244 @@
     <sheet name="10. Reviewing Performance" sheetId="10" state="visible" r:id="rId11"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="72">
   <si>
-    <t>What is the established velocity of the team?</t>
+    <t xml:space="preserve">What is the established velocity of the team?</t>
   </si>
   <si>
-    <t>Part 1</t>
+    <t xml:space="preserve">Part 1</t>
   </si>
   <si>
-    <t>Sprint 1</t>
+    <t xml:space="preserve">Sprint 1</t>
   </si>
   <si>
-    <t>Sprint 2</t>
+    <t xml:space="preserve">Sprint 2</t>
   </si>
   <si>
-    <t>Sprint 3</t>
+    <t xml:space="preserve">Sprint 3</t>
   </si>
   <si>
-    <t>Total</t>
+    <t xml:space="preserve">Total</t>
   </si>
   <si>
-    <t>Avg</t>
+    <t xml:space="preserve">Avg</t>
   </si>
   <si>
-    <t>How many sprints will it take to complete all the work?</t>
+    <t xml:space="preserve">How many sprints will it take to complete all the work?</t>
   </si>
   <si>
-    <t>Part 2</t>
+    <t xml:space="preserve">Part 2</t>
   </si>
   <si>
-    <t>Velocity</t>
+    <t xml:space="preserve">Velocity</t>
   </si>
   <si>
-    <t>Story Points</t>
+    <t xml:space="preserve">Story Points</t>
   </si>
   <si>
-    <t>Sprints</t>
+    <t xml:space="preserve">Sprints</t>
   </si>
   <si>
-    <t>Answer</t>
+    <t xml:space="preserve">Answer</t>
   </si>
   <si>
-    <t>What is the escaped defects % for team 1 and team 2</t>
+    <t xml:space="preserve">What is the escaped defects % for team 1 and team 2</t>
   </si>
   <si>
-    <t>Team 1 Environment</t>
+    <t xml:space="preserve">Team 1 Environment</t>
   </si>
   <si>
-    <t># of bugs</t>
+    <t xml:space="preserve"># of bugs</t>
   </si>
   <si>
-    <t>% of bugs found</t>
+    <t xml:space="preserve">% of bugs found</t>
   </si>
   <si>
-    <t>Dev</t>
+    <t xml:space="preserve">Dev</t>
   </si>
   <si>
-    <t>Staging</t>
+    <t xml:space="preserve">Staging</t>
   </si>
   <si>
-    <t>Production</t>
+    <t xml:space="preserve">Production</t>
   </si>
   <si>
-    <t>Team 2 Environment</t>
+    <t xml:space="preserve">Team 2 Environment</t>
   </si>
   <si>
-    <t>Use the data below and create at least three charts that will help the team answer the following questions:
+    <t xml:space="preserve">Use the data below and create at least three charts that will help the team answer the following questions:
 - Is the team delivering consistently?
 - Is the team's original delivery estimate accurate?
 - How many story points is the team delivering in each sprint?
 - What should the team commit to deliver in future sprints?</t>
   </si>
   <si>
-    <t>Sprint</t>
+    <t xml:space="preserve">Sprint</t>
   </si>
   <si>
-    <t>Story Point Completed</t>
+    <t xml:space="preserve">Story Point Completed</t>
   </si>
   <si>
-    <t>Points remaining</t>
+    <t xml:space="preserve">Points remaining</t>
   </si>
   <si>
-    <t>Cumulative Points Completed</t>
+    <t xml:space="preserve">Cumulative Points Completed</t>
   </si>
   <si>
-    <t>Sprint 0</t>
+    <t xml:space="preserve">Sprint 0</t>
   </si>
   <si>
-    <t>Sprint 4</t>
+    <t xml:space="preserve">Sprint 4</t>
   </si>
   <si>
-    <t>Use the data below to create a Committed vs Delivered Chart</t>
+    <t xml:space="preserve">Use the data below to create a Committed vs Delivered Chart</t>
   </si>
   <si>
-    <t>Committed</t>
+    <t xml:space="preserve">Committed</t>
   </si>
   <si>
-    <t>Delivered</t>
+    <t xml:space="preserve">Delivered</t>
   </si>
   <si>
-    <t>% Committed vs Delivered</t>
+    <t xml:space="preserve">% Committed vs Delivered</t>
   </si>
   <si>
-    <t>Sprint 5</t>
+    <t xml:space="preserve">Sprint 5</t>
   </si>
   <si>
-    <t>Sprint 6</t>
+    <t xml:space="preserve">Sprint 6</t>
   </si>
   <si>
-    <t>Create Chart Below</t>
+    <t xml:space="preserve">Create Chart Below</t>
   </si>
   <si>
-    <t>Use the provided Metrics below to figure out and create the following:
+    <t xml:space="preserve">Use the provided Metrics below to figure out and create the following:
 - Burn Down &amp; Chart
 - Burn Up &amp; Chart
 - Average Velocity over 5 Sprints
 - Expected Completion Sprint (BVIR)</t>
   </si>
   <si>
-    <t>Committed Story Points</t>
+    <t xml:space="preserve">Committed Story Points</t>
   </si>
   <si>
-    <t>Delivered Story Points</t>
+    <t xml:space="preserve">Delivered Story Points</t>
   </si>
   <si>
-    <t>Remaining Story Points</t>
+    <t xml:space="preserve">Remaining Story Points</t>
   </si>
   <si>
-    <t>Cummulative Story Points Completed</t>
+    <t xml:space="preserve">Cummulative Story Points Completed</t>
   </si>
   <si>
-    <t>Average</t>
+    <t xml:space="preserve">Average</t>
   </si>
   <si>
-    <t>Burn Down</t>
+    <t xml:space="preserve">Burn Down</t>
   </si>
   <si>
-    <t>Burn up Chart</t>
+    <t xml:space="preserve">Burn up Chart</t>
   </si>
   <si>
-    <t>Velocity Chart</t>
+    <t xml:space="preserve">Velocity Chart</t>
   </si>
   <si>
-    <t>Always round down value = 21</t>
+    <t xml:space="preserve">Always round down value = 21</t>
   </si>
   <si>
-    <t>BVIR</t>
+    <t xml:space="preserve">BVIR</t>
   </si>
   <si>
-    <t>Create a BVIR below that helps to show the expected completion sprint using charts from above. 
+    <t xml:space="preserve">Create a BVIR below that helps to show the expected completion sprint using charts from above. 
 You can copy them here to Create your BVIR. If you want to add text, do so in the cells surrounding the space below.</t>
   </si>
   <si>
-    <t>Use the data below to complete the following:
+    <t xml:space="preserve">Use the data below to complete the following:
 - Burn Down Metrics &amp; Chart
 - Burn Up Metrics &amp; Chart
 - Velocity Metrics &amp; Chart</t>
   </si>
   <si>
-    <t>Cumulative Story Points Completed</t>
+    <t xml:space="preserve">Cumulative Story Points Completed</t>
   </si>
   <si>
-    <t>Burn Down Chart</t>
+    <t xml:space="preserve">Burn Down Chart</t>
   </si>
   <si>
-    <t>Burn Up Chart</t>
+    <t xml:space="preserve">Burn Up Chart</t>
   </si>
   <si>
-    <t>Average Velocity</t>
+    <t xml:space="preserve">Average Velocity</t>
   </si>
   <si>
-    <t>Create a chart to display the quality rate over time</t>
+    <t xml:space="preserve">Create a chart to display the quality rate over time</t>
   </si>
   <si>
-    <t>Month</t>
+    <t xml:space="preserve">Month</t>
   </si>
   <si>
-    <t>Quality Rate</t>
+    <t xml:space="preserve">Quality Rate</t>
   </si>
   <si>
-    <t>Goal</t>
+    <t xml:space="preserve">Goal</t>
   </si>
   <si>
-    <t>High</t>
+    <t xml:space="preserve">High</t>
   </si>
   <si>
-    <t>January</t>
+    <t xml:space="preserve">January</t>
   </si>
   <si>
-    <t>February</t>
+    <t xml:space="preserve">February</t>
   </si>
   <si>
-    <t>March</t>
+    <t xml:space="preserve">March</t>
   </si>
   <si>
-    <t>April</t>
+    <t xml:space="preserve">April</t>
   </si>
   <si>
-    <t>May</t>
+    <t xml:space="preserve">May</t>
   </si>
   <si>
-    <t>June</t>
+    <t xml:space="preserve">June</t>
   </si>
   <si>
-    <t>Quality Metrics Chart</t>
+    <t xml:space="preserve">Quality Metrics Chart</t>
   </si>
   <si>
-    <t>Create a Quality chart and a Velocity chart</t>
+    <t xml:space="preserve">Create selecting Month, Quality Rate and Goal. All the rest is default. If you use MS check: https://classroom.udacity.com/nanodegrees/nd144/parts/cd0006/modules/859eb994-ce9d-407a-a141-e3efeba6541f/lessons/b7f54535-7631-4b68-a0eb-089e7e2047e2/concepts/8483c9ac-e70f-4f51-8b8f-a6647278f225</t>
   </si>
   <si>
-    <t>Quality Chart</t>
+    <t xml:space="preserve">Create a Quality chart and a Velocity chart</t>
   </si>
   <si>
-    <t>Story Points Completed</t>
+    <t xml:space="preserve">Quality Chart</t>
   </si>
   <si>
-    <t>Story Points Remaining</t>
+    <t xml:space="preserve">Story Points Completed</t>
   </si>
   <si>
-    <t>Use the data to create one or more charts to communicate what is currently happening with the project. 
+    <t xml:space="preserve">Story Points Remaining</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use the data to create one or more charts to communicate what is currently happening with the project. 
 CHALLENGE!  Can you use both data tables in one chart?</t>
   </si>
   <si>
-    <t>Chart(s)</t>
+    <t xml:space="preserve">Chart(s)</t>
   </si>
   <si>
-    <t>Use the data provided by the Product Owner to create a Committed vs Delivered Chart</t>
+    <t xml:space="preserve">Use the data provided by the Product Owner to create a Committed vs Delivered Chart</t>
   </si>
 </sst>
 </file>
@@ -257,17 +265,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
     <numFmt numFmtId="166" formatCode="0%"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -290,14 +297,12 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -305,27 +310,23 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Roboto"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -339,11 +340,7 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="13"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
+      <b val="true"/>
       <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -655,12 +652,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -728,18 +725,21 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
   <c:chart>
     <c:title>
       <c:tx>
         <c:rich>
-          <a:bodyPr/>
+          <a:bodyPr rot="0"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr b="1" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="1" sz="1300">
+              <a:rPr b="1" sz="1300" spc="-1" strike="noStrike">
                 <a:latin typeface="Arial"/>
               </a:rPr>
               <a:t>Burn Dowh Chart</a:t>
@@ -747,13 +747,20 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -761,10 +768,36 @@
             <a:solidFill>
               <a:srgbClr val="004586"/>
             </a:solidFill>
-            <a:ln>
+            <a:ln w="0">
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'3. Using Metrics'!$A$3:$A$7</c:f>
@@ -814,34 +847,48 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="18158"/>
-        <c:axId val="6280"/>
+        <c:overlap val="0"/>
+        <c:axId val="82859702"/>
+        <c:axId val="50855160"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="18158"/>
+        <c:axId val="82859702"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln>
+          <a:ln w="0">
             <a:solidFill>
               <a:srgbClr val="b3b3b3"/>
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="6280"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="50855160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="6280"/>
+        <c:axId val="50855160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -849,29 +896,42 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:ln>
+            <a:ln w="0">
               <a:solidFill>
                 <a:srgbClr val="b3b3b3"/>
               </a:solidFill>
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln>
+          <a:ln w="0">
             <a:solidFill>
               <a:srgbClr val="b3b3b3"/>
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="18158"/>
-        <c:crossesAt val="0"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="82859702"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="0">
           <a:solidFill>
             <a:srgbClr val="b3b3b3"/>
           </a:solidFill>
@@ -883,18 +943,30 @@
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
@@ -904,18 +976,21 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
   <c:chart>
     <c:title>
       <c:tx>
         <c:rich>
-          <a:bodyPr/>
+          <a:bodyPr rot="0"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr b="1" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="1" sz="1300">
+              <a:rPr b="1" sz="1300" spc="-1" strike="noStrike">
                 <a:latin typeface="Arial"/>
               </a:rPr>
               <a:t>Burn Up Chart</a:t>
@@ -923,13 +998,20 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -937,10 +1019,36 @@
             <a:solidFill>
               <a:srgbClr val="004586"/>
             </a:solidFill>
-            <a:ln>
+            <a:ln w="0">
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'3. Using Metrics'!$A$3:$A$7</c:f>
@@ -990,34 +1098,48 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="23115"/>
-        <c:axId val="26688"/>
+        <c:overlap val="0"/>
+        <c:axId val="15669312"/>
+        <c:axId val="4446592"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="23115"/>
+        <c:axId val="15669312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln>
+          <a:ln w="0">
             <a:solidFill>
               <a:srgbClr val="b3b3b3"/>
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="26688"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="4446592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="26688"/>
+        <c:axId val="4446592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1025,29 +1147,42 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:ln>
+            <a:ln w="0">
               <a:solidFill>
                 <a:srgbClr val="b3b3b3"/>
               </a:solidFill>
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln>
+          <a:ln w="0">
             <a:solidFill>
               <a:srgbClr val="b3b3b3"/>
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="23115"/>
-        <c:crossesAt val="0"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="15669312"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="0">
           <a:solidFill>
             <a:srgbClr val="b3b3b3"/>
           </a:solidFill>
@@ -1059,18 +1194,30 @@
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
@@ -1080,18 +1227,21 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
   <c:chart>
     <c:title>
       <c:tx>
         <c:rich>
-          <a:bodyPr/>
+          <a:bodyPr rot="0"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr b="1" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="1" sz="1300">
+              <a:rPr b="1" sz="1300" spc="-1" strike="noStrike">
                 <a:latin typeface="Arial"/>
               </a:rPr>
               <a:t>% Committed vs Delivered</a:t>
@@ -1099,13 +1249,20 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1115,7 +1272,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Committed</c:v>
+                  <c:v>'committed'</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1124,10 +1281,36 @@
             <a:solidFill>
               <a:srgbClr val="004586"/>
             </a:solidFill>
-            <a:ln>
+            <a:ln w="0">
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'4. Continuous Improvement'!$A$3:$A$8</c:f>
@@ -1191,7 +1374,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Delivered</c:v>
+                  <c:v>'delivered'</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1200,10 +1383,36 @@
             <a:solidFill>
               <a:srgbClr val="ff420e"/>
             </a:solidFill>
-            <a:ln>
+            <a:ln w="0">
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'4. Continuous Improvement'!$A$3:$A$8</c:f>
@@ -1259,34 +1468,48 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="8154"/>
-        <c:axId val="785"/>
+        <c:overlap val="0"/>
+        <c:axId val="60784883"/>
+        <c:axId val="24771248"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="8154"/>
+        <c:axId val="60784883"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln>
+          <a:ln w="0">
             <a:solidFill>
               <a:srgbClr val="b3b3b3"/>
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="785"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="24771248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="785"/>
+        <c:axId val="24771248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1294,29 +1517,42 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:ln>
+            <a:ln w="0">
               <a:solidFill>
                 <a:srgbClr val="b3b3b3"/>
               </a:solidFill>
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln>
+          <a:ln w="0">
             <a:solidFill>
               <a:srgbClr val="b3b3b3"/>
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="8154"/>
-        <c:crossesAt val="0"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="60784883"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="0">
           <a:solidFill>
             <a:srgbClr val="b3b3b3"/>
           </a:solidFill>
@@ -1328,18 +1564,30 @@
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
@@ -1349,18 +1597,21 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
   <c:chart>
     <c:title>
       <c:tx>
         <c:rich>
-          <a:bodyPr/>
+          <a:bodyPr rot="0"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr b="1" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300">
+              <a:rPr b="1" sz="1300" spc="-1" strike="noStrike">
                 <a:latin typeface="Arial"/>
               </a:rPr>
               <a:t>Burn Down Chart</a:t>
@@ -1368,13 +1619,20 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1393,10 +1651,36 @@
             <a:solidFill>
               <a:srgbClr val="004586"/>
             </a:solidFill>
-            <a:ln>
+            <a:ln w="0">
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'5. Simple BVIR'!$A$3:$A$8</c:f>
@@ -1452,34 +1736,48 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="28683"/>
-        <c:axId val="1838"/>
+        <c:overlap val="0"/>
+        <c:axId val="6763576"/>
+        <c:axId val="66830575"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="28683"/>
+        <c:axId val="6763576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln>
+          <a:ln w="0">
             <a:solidFill>
               <a:srgbClr val="b3b3b3"/>
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1838"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="66830575"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1838"/>
+        <c:axId val="66830575"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1487,7 +1785,7 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:ln>
+            <a:ln w="0">
               <a:solidFill>
                 <a:srgbClr val="b3b3b3"/>
               </a:solidFill>
@@ -1497,14 +1795,16 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr/>
+              <a:bodyPr rot="-5400000"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900">
+                  <a:rPr b="1" sz="900" spc="-1" strike="noStrike">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Story point remaining</a:t>
@@ -1512,24 +1812,43 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln>
+          <a:ln w="0">
             <a:solidFill>
               <a:srgbClr val="b3b3b3"/>
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="28683"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="6763576"/>
         <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="0">
           <a:solidFill>
             <a:srgbClr val="b3b3b3"/>
           </a:solidFill>
@@ -1541,18 +1860,30 @@
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
@@ -1562,18 +1893,21 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
   <c:chart>
     <c:title>
       <c:tx>
         <c:rich>
-          <a:bodyPr/>
+          <a:bodyPr rot="0"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr b="1" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300">
+              <a:rPr b="1" sz="1300" spc="-1" strike="noStrike">
                 <a:latin typeface="Arial"/>
               </a:rPr>
               <a:t>Burn Up Chart</a:t>
@@ -1581,13 +1915,20 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1606,10 +1947,36 @@
             <a:solidFill>
               <a:srgbClr val="004586"/>
             </a:solidFill>
-            <a:ln>
+            <a:ln w="0">
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'5. Simple BVIR'!$A$3:$A$8</c:f>
@@ -1665,34 +2032,48 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="450"/>
-        <c:axId val="894"/>
+        <c:overlap val="0"/>
+        <c:axId val="37355919"/>
+        <c:axId val="41661586"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="450"/>
+        <c:axId val="37355919"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln>
+          <a:ln w="0">
             <a:solidFill>
               <a:srgbClr val="b3b3b3"/>
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="894"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="41661586"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="894"/>
+        <c:axId val="41661586"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1700,7 +2081,7 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:ln>
+            <a:ln w="0">
               <a:solidFill>
                 <a:srgbClr val="b3b3b3"/>
               </a:solidFill>
@@ -1710,14 +2091,16 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr/>
+              <a:bodyPr rot="-5400000"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900">
+                  <a:rPr b="1" sz="900" spc="-1" strike="noStrike">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Story points completed</a:t>
@@ -1725,24 +2108,43 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln>
+          <a:ln w="0">
             <a:solidFill>
               <a:srgbClr val="b3b3b3"/>
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="450"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="37355919"/>
         <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="0">
           <a:solidFill>
             <a:srgbClr val="b3b3b3"/>
           </a:solidFill>
@@ -1754,18 +2156,30 @@
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
@@ -1775,18 +2189,21 @@
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
   <c:chart>
     <c:title>
       <c:tx>
         <c:rich>
-          <a:bodyPr/>
+          <a:bodyPr rot="0"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr b="1" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300">
+              <a:rPr b="1" sz="1300" spc="-1" strike="noStrike">
                 <a:latin typeface="Arial"/>
               </a:rPr>
               <a:t>Burn Down Chart</a:t>
@@ -1794,13 +2211,20 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1819,10 +2243,36 @@
             <a:solidFill>
               <a:srgbClr val="004586"/>
             </a:solidFill>
-            <a:ln>
+            <a:ln w="0">
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'6. Measuring Progress'!$A$3:$A$6</c:f>
@@ -1866,34 +2316,48 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="21908"/>
-        <c:axId val="5729"/>
+        <c:overlap val="0"/>
+        <c:axId val="79476059"/>
+        <c:axId val="52888766"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="21908"/>
+        <c:axId val="79476059"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln>
+          <a:ln w="0">
             <a:solidFill>
               <a:srgbClr val="b3b3b3"/>
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="5729"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="52888766"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="5729"/>
+        <c:axId val="52888766"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1901,7 +2365,7 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:ln>
+            <a:ln w="0">
               <a:solidFill>
                 <a:srgbClr val="b3b3b3"/>
               </a:solidFill>
@@ -1911,14 +2375,16 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr/>
+              <a:bodyPr rot="-5400000"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900">
+                  <a:rPr b="1" sz="900" spc="-1" strike="noStrike">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Story points remaining</a:t>
@@ -1926,24 +2392,43 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln>
+          <a:ln w="0">
             <a:solidFill>
               <a:srgbClr val="b3b3b3"/>
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="21908"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="79476059"/>
         <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="0">
           <a:solidFill>
             <a:srgbClr val="b3b3b3"/>
           </a:solidFill>
@@ -1955,18 +2440,30 @@
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
@@ -1976,18 +2473,21 @@
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
   <c:chart>
     <c:title>
       <c:tx>
         <c:rich>
-          <a:bodyPr/>
+          <a:bodyPr rot="0"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr b="1" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300">
+              <a:rPr b="1" sz="1300" spc="-1" strike="noStrike">
                 <a:latin typeface="Arial"/>
               </a:rPr>
               <a:t>Committed Vs Delivered</a:t>
@@ -1995,13 +2495,20 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -2020,10 +2527,36 @@
             <a:solidFill>
               <a:srgbClr val="004586"/>
             </a:solidFill>
-            <a:ln>
+            <a:ln w="0">
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'6. Measuring Progress'!$A$4:$A$6</c:f>
@@ -2078,10 +2611,36 @@
             <a:solidFill>
               <a:srgbClr val="ff420e"/>
             </a:solidFill>
-            <a:ln>
+            <a:ln w="0">
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'6. Measuring Progress'!$A$4:$A$6</c:f>
@@ -2119,34 +2678,48 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="14329"/>
-        <c:axId val="19366"/>
+        <c:overlap val="0"/>
+        <c:axId val="33251303"/>
+        <c:axId val="99709026"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="14329"/>
+        <c:axId val="33251303"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln>
+          <a:ln w="0">
             <a:solidFill>
               <a:srgbClr val="b3b3b3"/>
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="19366"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="99709026"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="19366"/>
+        <c:axId val="99709026"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2154,7 +2727,7 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:ln>
+            <a:ln w="0">
               <a:solidFill>
                 <a:srgbClr val="b3b3b3"/>
               </a:solidFill>
@@ -2164,14 +2737,16 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr/>
+              <a:bodyPr rot="-5400000"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900">
+                  <a:rPr b="1" sz="900" spc="-1" strike="noStrike">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Story points</a:t>
@@ -2179,24 +2754,43 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln>
+          <a:ln w="0">
             <a:solidFill>
               <a:srgbClr val="b3b3b3"/>
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="14329"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="33251303"/>
         <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="0">
           <a:solidFill>
             <a:srgbClr val="b3b3b3"/>
           </a:solidFill>
@@ -2208,18 +2802,30 @@
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
@@ -2229,18 +2835,21 @@
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
   <c:chart>
     <c:title>
       <c:tx>
         <c:rich>
-          <a:bodyPr/>
+          <a:bodyPr rot="0"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr b="1" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300">
+              <a:rPr b="1" sz="1300" spc="-1" strike="noStrike">
                 <a:latin typeface="Arial"/>
               </a:rPr>
               <a:t>Burn Up Chart</a:t>
@@ -2248,13 +2857,20 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -2273,10 +2889,36 @@
             <a:solidFill>
               <a:srgbClr val="004586"/>
             </a:solidFill>
-            <a:ln>
+            <a:ln w="0">
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'6. Measuring Progress'!$A$3:$A$6</c:f>
@@ -2320,34 +2962,48 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="31216"/>
-        <c:axId val="31504"/>
+        <c:overlap val="0"/>
+        <c:axId val="56915278"/>
+        <c:axId val="58187969"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="31216"/>
+        <c:axId val="56915278"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln>
+          <a:ln w="0">
             <a:solidFill>
               <a:srgbClr val="b3b3b3"/>
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="31504"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="58187969"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="31504"/>
+        <c:axId val="58187969"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2355,7 +3011,7 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:ln>
+            <a:ln w="0">
               <a:solidFill>
                 <a:srgbClr val="b3b3b3"/>
               </a:solidFill>
@@ -2365,14 +3021,16 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr/>
+              <a:bodyPr rot="-5400000"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900">
+                  <a:rPr b="1" sz="900" spc="-1" strike="noStrike">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Story points</a:t>
@@ -2380,24 +3038,43 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln>
+          <a:ln w="0">
             <a:solidFill>
               <a:srgbClr val="b3b3b3"/>
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="31216"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="56915278"/>
         <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="0">
           <a:solidFill>
             <a:srgbClr val="b3b3b3"/>
           </a:solidFill>
@@ -2409,18 +3086,372 @@
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'7. Quality Metrics'!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Quality Rate</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'7. Quality Metrics'!$A$3:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>January</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>February</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>March</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>April</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>May</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>June</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'7. Quality Metrics'!$B$3:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.983</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.981</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.965</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'7. Quality Metrics'!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Goal</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'7. Quality Metrics'!$A$3:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>January</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>February</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>March</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>April</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>May</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>June</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'7. Quality Metrics'!$C$3:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.98</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="100"/>
+        <c:overlap val="0"/>
+        <c:axId val="18533400"/>
+        <c:axId val="6043803"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="18533400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="6043803"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="6043803"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="18533400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="0">
       <a:noFill/>
     </a:ln>
   </c:spPr>
@@ -2432,7 +3463,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>80280</xdr:colOff>
+      <xdr:colOff>80640</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>22680</xdr:rowOff>
     </xdr:from>
@@ -2440,7 +3471,7 @@
       <xdr:col>15</xdr:col>
       <xdr:colOff>496440</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>44640</xdr:rowOff>
+      <xdr:rowOff>44280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2448,8 +3479,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5871240" y="1267200"/>
-        <a:ext cx="5753880" cy="3238200"/>
+        <a:off x="5871600" y="1267200"/>
+        <a:ext cx="5753520" cy="3237840"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2462,9 +3493,9 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>110520</xdr:colOff>
+      <xdr:colOff>110880</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>35640</xdr:rowOff>
+      <xdr:rowOff>36000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
@@ -2478,8 +3509,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5901480" y="4877280"/>
-        <a:ext cx="5763600" cy="3238200"/>
+        <a:off x="5901840" y="4877640"/>
+        <a:ext cx="5763240" cy="3237840"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2503,9 +3534,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>57240</xdr:colOff>
+      <xdr:colOff>56880</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>25920</xdr:rowOff>
+      <xdr:rowOff>25560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2513,8 +3544,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="117360" y="2934360"/>
-        <a:ext cx="5756760" cy="3238200"/>
+        <a:off x="117360" y="2843640"/>
+        <a:ext cx="5756400" cy="3237840"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2532,15 +3563,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>279000</xdr:colOff>
+      <xdr:colOff>279360</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>390600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>113760</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>114480</xdr:rowOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>24120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2548,8 +3579,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8352720" y="390600"/>
-        <a:ext cx="5765760" cy="3238560"/>
+        <a:off x="8353080" y="390600"/>
+        <a:ext cx="5765400" cy="3238200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2562,7 +3593,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>258840</xdr:colOff>
+      <xdr:colOff>259200</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>28800</xdr:rowOff>
     </xdr:from>
@@ -2570,7 +3601,7 @@
       <xdr:col>18</xdr:col>
       <xdr:colOff>93600</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>9720</xdr:rowOff>
+      <xdr:rowOff>9360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2578,8 +3609,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8332560" y="3905280"/>
-        <a:ext cx="5765760" cy="3238560"/>
+        <a:off x="8332920" y="3814560"/>
+        <a:ext cx="5765400" cy="3238200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2599,13 +3630,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>56160</xdr:rowOff>
+      <xdr:rowOff>56520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1306440</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>95400</xdr:rowOff>
+      <xdr:colOff>1306080</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>57240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2613,8 +3644,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="0" y="2697480"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:off x="0" y="2568960"/>
+        <a:ext cx="5759280" cy="3239280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2633,9 +3664,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>47160</xdr:colOff>
-      <xdr:row>63</xdr:row>
-      <xdr:rowOff>30600</xdr:rowOff>
+      <xdr:colOff>46800</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>43200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2643,8 +3674,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="107640" y="10316160"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:off x="107640" y="9793800"/>
+        <a:ext cx="5759280" cy="3239280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2659,13 +3690,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>24480</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>40320</xdr:rowOff>
+      <xdr:rowOff>40680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1330920</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>54360</xdr:rowOff>
+      <xdr:colOff>1330560</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>41400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2673,8 +3704,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="24480" y="6275880"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:off x="24480" y="5982120"/>
+        <a:ext cx="5759280" cy="3239280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2687,26 +3718,60 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>306360</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>77040</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>261720</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>78120</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="306360" y="2594520"/>
+        <a:ext cx="5759640" cy="3239640"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z16"/>
+  <dimension ref="A1:Z14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="12.65625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.1674418604651"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.5906976744186"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="7.66046511627907"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.4976744186046"/>
-    <col collapsed="false" hidden="false" max="26" min="7" style="0" width="7.66046511627907"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="12.6651162790698"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="0" width="7.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="0" width="7.66"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="37" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3145,7 +4210,6 @@
       <c r="Y14" s="3"/>
       <c r="Z14" s="3"/>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:B1"/>
@@ -3155,7 +4219,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3164,30 +4228,30 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="12.65625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="9.82790697674419"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="13.6697674418605"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="12.5023255813953"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="14.9953488372093"/>
-    <col collapsed="false" hidden="false" max="26" min="5" style="10" width="7.66046511627907"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="10" width="12.6651162790698"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="9.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="13.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="12.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="5" style="10" width="7.66"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="10" width="12.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="38" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="18" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="18"/>
@@ -3261,7 +4325,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3270,23 +4334,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="12.65625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="32.3302325581395"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="13.1581395348837"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="16.4976744186046"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="10" width="12.6651162790698"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="32.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="13.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="16.5"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="10" width="12.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3419,7 +4483,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3428,25 +4492,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:18"/>
+  <dimension ref="A1:AMJ18"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="12.65625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="13.6697674418605"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="14.6697674418605"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="14.1581395348837"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="17"/>
-    <col collapsed="false" hidden="false" max="25" min="5" style="10" width="7.66046511627907"/>
-    <col collapsed="false" hidden="false" max="1025" min="26" style="10" width="12.6651162790698"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="13.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="14.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="14.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="5" style="10" width="7.66"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="26" style="10" width="12.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="98" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4614,7 +5678,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -4624,25 +5688,25 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="12.65625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="13.1581395348837"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="18.6651162790698"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="15.506976744186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="20.1674418604651"/>
-    <col collapsed="false" hidden="false" max="26" min="5" style="10" width="7.66046511627907"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="10" width="12.6651162790698"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="13.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="18.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="15.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="20.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="5" style="10" width="7.66"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="10" width="12.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4653,7 +5717,7 @@
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
     </row>
-    <row r="2" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="23" t="s">
         <v>22</v>
       </c>
@@ -4771,7 +5835,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -4781,26 +5845,26 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:45"/>
+  <dimension ref="A1:AMJ45"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B37" activeCellId="0" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="12.65625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="14.8325581395349"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="15.8325581395349"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="13.9953488372093"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="15.1627906976744"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="10" width="21.5023255813953"/>
-    <col collapsed="false" hidden="false" max="26" min="6" style="10" width="7.66046511627907"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="10" width="12.6651162790698"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="14.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="15.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="15.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="21.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="6" style="10" width="7.66"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="10" width="12.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="86" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5831,7 +6895,7 @@
       <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
     </row>
-    <row r="2" s="22" customFormat="true" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="22" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="23" t="s">
         <v>22</v>
       </c>
@@ -6545,7 +7609,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -6555,26 +7619,26 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:67"/>
+  <dimension ref="A1:AMJ96"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A67" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A71" activeCellId="0" sqref="A71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="18.5395348837209"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="18.8279069767442"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="20.1674418604651"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="17.6651162790698"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="10" width="21.5023255813953"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="10" width="18.5023255813954"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="10" width="10.8279069767442"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="18.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="18.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="20.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="17.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="21.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="10" width="18.5"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="10" width="10.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="66" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7605,7 +8669,7 @@
       <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
     </row>
-    <row r="2" s="22" customFormat="true" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="22" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="19" t="s">
         <v>22</v>
       </c>
@@ -7740,7 +8804,7 @@
       <c r="L6" s="0"/>
       <c r="M6" s="0"/>
     </row>
-    <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
         <v>40</v>
       </c>
@@ -7757,7 +8821,7 @@
       <c r="L7" s="0"/>
       <c r="M7" s="0"/>
     </row>
-    <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0"/>
       <c r="B8" s="0"/>
       <c r="C8" s="0"/>
@@ -7772,7 +8836,7 @@
       <c r="L8" s="0"/>
       <c r="M8" s="0"/>
     </row>
-    <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="30" t="s">
         <v>49</v>
       </c>
@@ -7789,7 +8853,7 @@
       <c r="L9" s="0"/>
       <c r="M9" s="0"/>
     </row>
-    <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0"/>
       <c r="B10" s="0"/>
       <c r="C10" s="0"/>
@@ -7834,7 +8898,7 @@
       <c r="L12" s="0"/>
       <c r="M12" s="0"/>
     </row>
-    <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0"/>
       <c r="B13" s="0"/>
       <c r="C13" s="0"/>
@@ -7849,7 +8913,7 @@
       <c r="L13" s="0"/>
       <c r="M13" s="0"/>
     </row>
-    <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0"/>
       <c r="B14" s="0"/>
       <c r="C14" s="0"/>
@@ -7864,7 +8928,7 @@
       <c r="L14" s="0"/>
       <c r="M14" s="0"/>
     </row>
-    <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0"/>
       <c r="B15" s="0"/>
       <c r="C15" s="0"/>
@@ -7879,7 +8943,7 @@
       <c r="L15" s="0"/>
       <c r="M15" s="0"/>
     </row>
-    <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0"/>
       <c r="B16" s="0"/>
       <c r="C16" s="0"/>
@@ -7894,7 +8958,7 @@
       <c r="L16" s="0"/>
       <c r="M16" s="0"/>
     </row>
-    <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0"/>
       <c r="B17" s="0"/>
       <c r="C17" s="0"/>
@@ -7924,7 +8988,7 @@
       <c r="L18" s="0"/>
       <c r="M18" s="0"/>
     </row>
-    <row r="19" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0"/>
       <c r="B19" s="0"/>
       <c r="C19" s="0"/>
@@ -7939,7 +9003,7 @@
       <c r="L19" s="0"/>
       <c r="M19" s="0"/>
     </row>
-    <row r="20" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0"/>
       <c r="B20" s="0"/>
       <c r="C20" s="0"/>
@@ -7954,7 +9018,7 @@
       <c r="L20" s="0"/>
       <c r="M20" s="0"/>
     </row>
-    <row r="21" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0"/>
       <c r="B21" s="0"/>
       <c r="C21" s="0"/>
@@ -7969,7 +9033,7 @@
       <c r="L21" s="0"/>
       <c r="M21" s="0"/>
     </row>
-    <row r="22" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0"/>
       <c r="B22" s="0"/>
       <c r="C22" s="0"/>
@@ -7984,7 +9048,7 @@
       <c r="L22" s="0"/>
       <c r="M22" s="0"/>
     </row>
-    <row r="23" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0"/>
       <c r="B23" s="0"/>
       <c r="C23" s="0"/>
@@ -7999,7 +9063,7 @@
       <c r="L23" s="0"/>
       <c r="M23" s="0"/>
     </row>
-    <row r="24" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0"/>
       <c r="B24" s="0"/>
       <c r="C24" s="0"/>
@@ -8029,7 +9093,7 @@
       <c r="L25" s="0"/>
       <c r="M25" s="0"/>
     </row>
-    <row r="26" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0"/>
       <c r="B26" s="0"/>
       <c r="C26" s="0"/>
@@ -8061,7 +9125,7 @@
       <c r="L27" s="0"/>
       <c r="M27" s="0"/>
     </row>
-    <row r="28" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0"/>
       <c r="B28" s="0"/>
       <c r="C28" s="0"/>
@@ -8076,7 +9140,7 @@
       <c r="L28" s="0"/>
       <c r="M28" s="0"/>
     </row>
-    <row r="29" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0"/>
       <c r="B29" s="0"/>
       <c r="C29" s="0"/>
@@ -8091,7 +9155,7 @@
       <c r="L29" s="0"/>
       <c r="M29" s="0"/>
     </row>
-    <row r="30" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0"/>
       <c r="B30" s="0"/>
       <c r="C30" s="0"/>
@@ -8106,7 +9170,7 @@
       <c r="L30" s="0"/>
       <c r="M30" s="0"/>
     </row>
-    <row r="31" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0"/>
       <c r="B31" s="0"/>
       <c r="C31" s="0"/>
@@ -8121,7 +9185,7 @@
       <c r="L31" s="0"/>
       <c r="M31" s="0"/>
     </row>
-    <row r="32" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0"/>
       <c r="B32" s="0"/>
       <c r="C32" s="0"/>
@@ -8136,7 +9200,7 @@
       <c r="L32" s="0"/>
       <c r="M32" s="0"/>
     </row>
-    <row r="33" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0"/>
       <c r="B33" s="0"/>
       <c r="C33" s="0"/>
@@ -8166,7 +9230,7 @@
       <c r="L34" s="0"/>
       <c r="M34" s="0"/>
     </row>
-    <row r="35" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0"/>
       <c r="B35" s="0"/>
       <c r="C35" s="0"/>
@@ -8181,7 +9245,7 @@
       <c r="L35" s="0"/>
       <c r="M35" s="0"/>
     </row>
-    <row r="36" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0"/>
       <c r="B36" s="0"/>
       <c r="C36" s="0"/>
@@ -8196,7 +9260,7 @@
       <c r="L36" s="0"/>
       <c r="M36" s="0"/>
     </row>
-    <row r="37" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0"/>
       <c r="B37" s="0"/>
       <c r="C37" s="0"/>
@@ -8211,7 +9275,7 @@
       <c r="L37" s="0"/>
       <c r="M37" s="0"/>
     </row>
-    <row r="38" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0"/>
       <c r="B38" s="0"/>
       <c r="C38" s="0"/>
@@ -8226,7 +9290,7 @@
       <c r="L38" s="0"/>
       <c r="M38" s="0"/>
     </row>
-    <row r="39" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0"/>
       <c r="B39" s="0"/>
       <c r="C39" s="0"/>
@@ -8241,7 +9305,7 @@
       <c r="L39" s="0"/>
       <c r="M39" s="0"/>
     </row>
-    <row r="40" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0"/>
       <c r="B40" s="0"/>
       <c r="C40" s="0"/>
@@ -8256,7 +9320,7 @@
       <c r="L40" s="0"/>
       <c r="M40" s="0"/>
     </row>
-    <row r="41" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0"/>
       <c r="B41" s="0"/>
       <c r="C41" s="0"/>
@@ -8271,7 +9335,7 @@
       <c r="L41" s="0"/>
       <c r="M41" s="0"/>
     </row>
-    <row r="42" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0"/>
       <c r="B42" s="0"/>
       <c r="C42" s="0"/>
@@ -8301,7 +9365,7 @@
       <c r="L43" s="0"/>
       <c r="M43" s="0"/>
     </row>
-    <row r="44" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0"/>
       <c r="B44" s="0"/>
       <c r="C44" s="0"/>
@@ -8316,7 +9380,7 @@
       <c r="L44" s="0"/>
       <c r="M44" s="0"/>
     </row>
-    <row r="45" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="30" t="s">
         <v>51</v>
       </c>
@@ -8333,7 +9397,7 @@
       <c r="L45" s="0"/>
       <c r="M45" s="0"/>
     </row>
-    <row r="46" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="n">
         <f aca="false">64/3</f>
         <v>21.3333333333333</v>
@@ -8353,7 +9417,7 @@
       <c r="L46" s="0"/>
       <c r="M46" s="0"/>
     </row>
-    <row r="47" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0"/>
       <c r="B47" s="0"/>
       <c r="C47" s="0"/>
@@ -8368,7 +9432,7 @@
       <c r="L47" s="0"/>
       <c r="M47" s="0"/>
     </row>
-    <row r="48" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0"/>
       <c r="B48" s="0"/>
       <c r="C48" s="0"/>
@@ -8383,7 +9447,7 @@
       <c r="L48" s="0"/>
       <c r="M48" s="0"/>
     </row>
-    <row r="49" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0"/>
       <c r="B49" s="0"/>
       <c r="C49" s="0"/>
@@ -8398,7 +9462,7 @@
       <c r="L49" s="0"/>
       <c r="M49" s="0"/>
     </row>
-    <row r="50" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0"/>
       <c r="B50" s="0"/>
       <c r="C50" s="0"/>
@@ -8413,7 +9477,7 @@
       <c r="L50" s="0"/>
       <c r="M50" s="0"/>
     </row>
-    <row r="51" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0"/>
       <c r="B51" s="0"/>
       <c r="C51" s="0"/>
@@ -8428,7 +9492,7 @@
       <c r="L51" s="0"/>
       <c r="M51" s="0"/>
     </row>
-    <row r="52" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0"/>
       <c r="B52" s="0"/>
       <c r="C52" s="0"/>
@@ -8443,7 +9507,7 @@
       <c r="L52" s="0"/>
       <c r="M52" s="0"/>
     </row>
-    <row r="53" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0"/>
       <c r="B53" s="0"/>
       <c r="C53" s="0"/>
@@ -8458,7 +9522,7 @@
       <c r="L53" s="0"/>
       <c r="M53" s="0"/>
     </row>
-    <row r="54" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0"/>
       <c r="B54" s="0"/>
       <c r="C54" s="0"/>
@@ -8473,7 +9537,7 @@
       <c r="L54" s="0"/>
       <c r="M54" s="0"/>
     </row>
-    <row r="55" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0"/>
       <c r="B55" s="0"/>
       <c r="C55" s="0"/>
@@ -8488,7 +9552,7 @@
       <c r="L55" s="0"/>
       <c r="M55" s="0"/>
     </row>
-    <row r="56" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0"/>
       <c r="B56" s="0"/>
       <c r="C56" s="0"/>
@@ -8503,7 +9567,7 @@
       <c r="L56" s="0"/>
       <c r="M56" s="0"/>
     </row>
-    <row r="57" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0"/>
       <c r="B57" s="0"/>
       <c r="C57" s="0"/>
@@ -8518,7 +9582,7 @@
       <c r="L57" s="0"/>
       <c r="M57" s="0"/>
     </row>
-    <row r="58" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0"/>
       <c r="B58" s="0"/>
       <c r="C58" s="0"/>
@@ -8533,7 +9597,7 @@
       <c r="L58" s="0"/>
       <c r="M58" s="0"/>
     </row>
-    <row r="59" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0"/>
       <c r="B59" s="0"/>
       <c r="C59" s="0"/>
@@ -8548,7 +9612,7 @@
       <c r="L59" s="0"/>
       <c r="M59" s="0"/>
     </row>
-    <row r="60" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0"/>
       <c r="B60" s="0"/>
       <c r="C60" s="0"/>
@@ -8563,7 +9627,7 @@
       <c r="L60" s="0"/>
       <c r="M60" s="0"/>
     </row>
-    <row r="61" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="30"/>
       <c r="B61" s="0"/>
       <c r="C61" s="0"/>
@@ -8578,7 +9642,7 @@
       <c r="L61" s="0"/>
       <c r="M61" s="0"/>
     </row>
-    <row r="62" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0"/>
       <c r="B62" s="0"/>
       <c r="C62" s="0"/>
@@ -8593,7 +9657,7 @@
       <c r="L62" s="0"/>
       <c r="M62" s="0"/>
     </row>
-    <row r="63" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0"/>
       <c r="B63" s="0"/>
       <c r="C63" s="0"/>
@@ -8608,7 +9672,7 @@
       <c r="L63" s="0"/>
       <c r="M63" s="0"/>
     </row>
-    <row r="64" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0"/>
       <c r="B64" s="0"/>
       <c r="C64" s="0"/>
@@ -8623,7 +9687,7 @@
       <c r="L64" s="0"/>
       <c r="M64" s="0"/>
     </row>
-    <row r="65" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0"/>
       <c r="B65" s="0"/>
       <c r="C65" s="0"/>
@@ -8638,7 +9702,7 @@
       <c r="L65" s="0"/>
       <c r="M65" s="0"/>
     </row>
-    <row r="66" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0"/>
       <c r="B66" s="0"/>
       <c r="C66" s="0"/>
@@ -8653,7 +9717,7 @@
       <c r="L66" s="0"/>
       <c r="M66" s="0"/>
     </row>
-    <row r="67" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="30" t="s">
         <v>45</v>
       </c>
@@ -8670,6 +9734,412 @@
       <c r="L67" s="31"/>
       <c r="M67" s="31"/>
     </row>
+    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B68" s="31"/>
+      <c r="C68" s="31"/>
+      <c r="D68" s="31"/>
+      <c r="E68" s="31"/>
+      <c r="F68" s="31"/>
+      <c r="G68" s="31"/>
+      <c r="H68" s="31"/>
+      <c r="I68" s="31"/>
+      <c r="J68" s="31"/>
+      <c r="K68" s="31"/>
+      <c r="L68" s="31"/>
+      <c r="M68" s="31"/>
+    </row>
+    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B69" s="31"/>
+      <c r="C69" s="31"/>
+      <c r="D69" s="31"/>
+      <c r="E69" s="31"/>
+      <c r="F69" s="31"/>
+      <c r="G69" s="31"/>
+      <c r="H69" s="31"/>
+      <c r="I69" s="31"/>
+      <c r="J69" s="31"/>
+      <c r="K69" s="31"/>
+      <c r="L69" s="31"/>
+      <c r="M69" s="31"/>
+    </row>
+    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B70" s="31"/>
+      <c r="C70" s="31"/>
+      <c r="D70" s="31"/>
+      <c r="E70" s="31"/>
+      <c r="F70" s="31"/>
+      <c r="G70" s="31"/>
+      <c r="H70" s="31"/>
+      <c r="I70" s="31"/>
+      <c r="J70" s="31"/>
+      <c r="K70" s="31"/>
+      <c r="L70" s="31"/>
+      <c r="M70" s="31"/>
+    </row>
+    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B71" s="31"/>
+      <c r="C71" s="31"/>
+      <c r="D71" s="31"/>
+      <c r="E71" s="31"/>
+      <c r="F71" s="31"/>
+      <c r="G71" s="31"/>
+      <c r="H71" s="31"/>
+      <c r="I71" s="31"/>
+      <c r="J71" s="31"/>
+      <c r="K71" s="31"/>
+      <c r="L71" s="31"/>
+      <c r="M71" s="31"/>
+    </row>
+    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B72" s="31"/>
+      <c r="C72" s="31"/>
+      <c r="D72" s="31"/>
+      <c r="E72" s="31"/>
+      <c r="F72" s="31"/>
+      <c r="G72" s="31"/>
+      <c r="H72" s="31"/>
+      <c r="I72" s="31"/>
+      <c r="J72" s="31"/>
+      <c r="K72" s="31"/>
+      <c r="L72" s="31"/>
+      <c r="M72" s="31"/>
+    </row>
+    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B73" s="31"/>
+      <c r="C73" s="31"/>
+      <c r="D73" s="31"/>
+      <c r="E73" s="31"/>
+      <c r="F73" s="31"/>
+      <c r="G73" s="31"/>
+      <c r="H73" s="31"/>
+      <c r="I73" s="31"/>
+      <c r="J73" s="31"/>
+      <c r="K73" s="31"/>
+      <c r="L73" s="31"/>
+      <c r="M73" s="31"/>
+    </row>
+    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B74" s="31"/>
+      <c r="C74" s="31"/>
+      <c r="D74" s="31"/>
+      <c r="E74" s="31"/>
+      <c r="F74" s="31"/>
+      <c r="G74" s="31"/>
+      <c r="H74" s="31"/>
+      <c r="I74" s="31"/>
+      <c r="J74" s="31"/>
+      <c r="K74" s="31"/>
+      <c r="L74" s="31"/>
+      <c r="M74" s="31"/>
+    </row>
+    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B75" s="31"/>
+      <c r="C75" s="31"/>
+      <c r="D75" s="31"/>
+      <c r="E75" s="31"/>
+      <c r="F75" s="31"/>
+      <c r="G75" s="31"/>
+      <c r="H75" s="31"/>
+      <c r="I75" s="31"/>
+      <c r="J75" s="31"/>
+      <c r="K75" s="31"/>
+      <c r="L75" s="31"/>
+      <c r="M75" s="31"/>
+    </row>
+    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B76" s="31"/>
+      <c r="C76" s="31"/>
+      <c r="D76" s="31"/>
+      <c r="E76" s="31"/>
+      <c r="F76" s="31"/>
+      <c r="G76" s="31"/>
+      <c r="H76" s="31"/>
+      <c r="I76" s="31"/>
+      <c r="J76" s="31"/>
+      <c r="K76" s="31"/>
+      <c r="L76" s="31"/>
+      <c r="M76" s="31"/>
+    </row>
+    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B77" s="31"/>
+      <c r="C77" s="31"/>
+      <c r="D77" s="31"/>
+      <c r="E77" s="31"/>
+      <c r="F77" s="31"/>
+      <c r="G77" s="31"/>
+      <c r="H77" s="31"/>
+      <c r="I77" s="31"/>
+      <c r="J77" s="31"/>
+      <c r="K77" s="31"/>
+      <c r="L77" s="31"/>
+      <c r="M77" s="31"/>
+    </row>
+    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B78" s="31"/>
+      <c r="C78" s="31"/>
+      <c r="D78" s="31"/>
+      <c r="E78" s="31"/>
+      <c r="F78" s="31"/>
+      <c r="G78" s="31"/>
+      <c r="H78" s="31"/>
+      <c r="I78" s="31"/>
+      <c r="J78" s="31"/>
+      <c r="K78" s="31"/>
+      <c r="L78" s="31"/>
+      <c r="M78" s="31"/>
+    </row>
+    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B79" s="31"/>
+      <c r="C79" s="31"/>
+      <c r="D79" s="31"/>
+      <c r="E79" s="31"/>
+      <c r="F79" s="31"/>
+      <c r="G79" s="31"/>
+      <c r="H79" s="31"/>
+      <c r="I79" s="31"/>
+      <c r="J79" s="31"/>
+      <c r="K79" s="31"/>
+      <c r="L79" s="31"/>
+      <c r="M79" s="31"/>
+    </row>
+    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B80" s="31"/>
+      <c r="C80" s="31"/>
+      <c r="D80" s="31"/>
+      <c r="E80" s="31"/>
+      <c r="F80" s="31"/>
+      <c r="G80" s="31"/>
+      <c r="H80" s="31"/>
+      <c r="I80" s="31"/>
+      <c r="J80" s="31"/>
+      <c r="K80" s="31"/>
+      <c r="L80" s="31"/>
+      <c r="M80" s="31"/>
+    </row>
+    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B81" s="31"/>
+      <c r="C81" s="31"/>
+      <c r="D81" s="31"/>
+      <c r="E81" s="31"/>
+      <c r="F81" s="31"/>
+      <c r="G81" s="31"/>
+      <c r="H81" s="31"/>
+      <c r="I81" s="31"/>
+      <c r="J81" s="31"/>
+      <c r="K81" s="31"/>
+      <c r="L81" s="31"/>
+      <c r="M81" s="31"/>
+    </row>
+    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B82" s="31"/>
+      <c r="C82" s="31"/>
+      <c r="D82" s="31"/>
+      <c r="E82" s="31"/>
+      <c r="F82" s="31"/>
+      <c r="G82" s="31"/>
+      <c r="H82" s="31"/>
+      <c r="I82" s="31"/>
+      <c r="J82" s="31"/>
+      <c r="K82" s="31"/>
+      <c r="L82" s="31"/>
+      <c r="M82" s="31"/>
+    </row>
+    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B83" s="31"/>
+      <c r="C83" s="31"/>
+      <c r="D83" s="31"/>
+      <c r="E83" s="31"/>
+      <c r="F83" s="31"/>
+      <c r="G83" s="31"/>
+      <c r="H83" s="31"/>
+      <c r="I83" s="31"/>
+      <c r="J83" s="31"/>
+      <c r="K83" s="31"/>
+      <c r="L83" s="31"/>
+      <c r="M83" s="31"/>
+    </row>
+    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B84" s="31"/>
+      <c r="C84" s="31"/>
+      <c r="D84" s="31"/>
+      <c r="E84" s="31"/>
+      <c r="F84" s="31"/>
+      <c r="G84" s="31"/>
+      <c r="H84" s="31"/>
+      <c r="I84" s="31"/>
+      <c r="J84" s="31"/>
+      <c r="K84" s="31"/>
+      <c r="L84" s="31"/>
+      <c r="M84" s="31"/>
+    </row>
+    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B85" s="31"/>
+      <c r="C85" s="31"/>
+      <c r="D85" s="31"/>
+      <c r="E85" s="31"/>
+      <c r="F85" s="31"/>
+      <c r="G85" s="31"/>
+      <c r="H85" s="31"/>
+      <c r="I85" s="31"/>
+      <c r="J85" s="31"/>
+      <c r="K85" s="31"/>
+      <c r="L85" s="31"/>
+      <c r="M85" s="31"/>
+    </row>
+    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B86" s="31"/>
+      <c r="C86" s="31"/>
+      <c r="D86" s="31"/>
+      <c r="E86" s="31"/>
+      <c r="F86" s="31"/>
+      <c r="G86" s="31"/>
+      <c r="H86" s="31"/>
+      <c r="I86" s="31"/>
+      <c r="J86" s="31"/>
+      <c r="K86" s="31"/>
+      <c r="L86" s="31"/>
+      <c r="M86" s="31"/>
+    </row>
+    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B87" s="31"/>
+      <c r="C87" s="31"/>
+      <c r="D87" s="31"/>
+      <c r="E87" s="31"/>
+      <c r="F87" s="31"/>
+      <c r="G87" s="31"/>
+      <c r="H87" s="31"/>
+      <c r="I87" s="31"/>
+      <c r="J87" s="31"/>
+      <c r="K87" s="31"/>
+      <c r="L87" s="31"/>
+      <c r="M87" s="31"/>
+    </row>
+    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B88" s="31"/>
+      <c r="C88" s="31"/>
+      <c r="D88" s="31"/>
+      <c r="E88" s="31"/>
+      <c r="F88" s="31"/>
+      <c r="G88" s="31"/>
+      <c r="H88" s="31"/>
+      <c r="I88" s="31"/>
+      <c r="J88" s="31"/>
+      <c r="K88" s="31"/>
+      <c r="L88" s="31"/>
+      <c r="M88" s="31"/>
+    </row>
+    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B89" s="31"/>
+      <c r="C89" s="31"/>
+      <c r="D89" s="31"/>
+      <c r="E89" s="31"/>
+      <c r="F89" s="31"/>
+      <c r="G89" s="31"/>
+      <c r="H89" s="31"/>
+      <c r="I89" s="31"/>
+      <c r="J89" s="31"/>
+      <c r="K89" s="31"/>
+      <c r="L89" s="31"/>
+      <c r="M89" s="31"/>
+    </row>
+    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B90" s="31"/>
+      <c r="C90" s="31"/>
+      <c r="D90" s="31"/>
+      <c r="E90" s="31"/>
+      <c r="F90" s="31"/>
+      <c r="G90" s="31"/>
+      <c r="H90" s="31"/>
+      <c r="I90" s="31"/>
+      <c r="J90" s="31"/>
+      <c r="K90" s="31"/>
+      <c r="L90" s="31"/>
+      <c r="M90" s="31"/>
+    </row>
+    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B91" s="31"/>
+      <c r="C91" s="31"/>
+      <c r="D91" s="31"/>
+      <c r="E91" s="31"/>
+      <c r="F91" s="31"/>
+      <c r="G91" s="31"/>
+      <c r="H91" s="31"/>
+      <c r="I91" s="31"/>
+      <c r="J91" s="31"/>
+      <c r="K91" s="31"/>
+      <c r="L91" s="31"/>
+      <c r="M91" s="31"/>
+    </row>
+    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B92" s="31"/>
+      <c r="C92" s="31"/>
+      <c r="D92" s="31"/>
+      <c r="E92" s="31"/>
+      <c r="F92" s="31"/>
+      <c r="G92" s="31"/>
+      <c r="H92" s="31"/>
+      <c r="I92" s="31"/>
+      <c r="J92" s="31"/>
+      <c r="K92" s="31"/>
+      <c r="L92" s="31"/>
+      <c r="M92" s="31"/>
+    </row>
+    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B93" s="31"/>
+      <c r="C93" s="31"/>
+      <c r="D93" s="31"/>
+      <c r="E93" s="31"/>
+      <c r="F93" s="31"/>
+      <c r="G93" s="31"/>
+      <c r="H93" s="31"/>
+      <c r="I93" s="31"/>
+      <c r="J93" s="31"/>
+      <c r="K93" s="31"/>
+      <c r="L93" s="31"/>
+      <c r="M93" s="31"/>
+    </row>
+    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B94" s="31"/>
+      <c r="C94" s="31"/>
+      <c r="D94" s="31"/>
+      <c r="E94" s="31"/>
+      <c r="F94" s="31"/>
+      <c r="G94" s="31"/>
+      <c r="H94" s="31"/>
+      <c r="I94" s="31"/>
+      <c r="J94" s="31"/>
+      <c r="K94" s="31"/>
+      <c r="L94" s="31"/>
+      <c r="M94" s="31"/>
+    </row>
+    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B95" s="31"/>
+      <c r="C95" s="31"/>
+      <c r="D95" s="31"/>
+      <c r="E95" s="31"/>
+      <c r="F95" s="31"/>
+      <c r="G95" s="31"/>
+      <c r="H95" s="31"/>
+      <c r="I95" s="31"/>
+      <c r="J95" s="31"/>
+      <c r="K95" s="31"/>
+      <c r="L95" s="31"/>
+      <c r="M95" s="31"/>
+    </row>
+    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B96" s="31"/>
+      <c r="C96" s="31"/>
+      <c r="D96" s="31"/>
+      <c r="E96" s="31"/>
+      <c r="F96" s="31"/>
+      <c r="G96" s="31"/>
+      <c r="H96" s="31"/>
+      <c r="I96" s="31"/>
+      <c r="J96" s="31"/>
+      <c r="K96" s="31"/>
+      <c r="L96" s="31"/>
+      <c r="M96" s="31"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:F1"/>
@@ -8677,7 +10147,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -8687,25 +10157,25 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N23" activeCellId="0" sqref="N23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="12.65625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="13.6697674418605"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="13.5023255813954"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="12.8325581395349"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="12.0046511627907"/>
-    <col collapsed="false" hidden="false" max="26" min="5" style="10" width="7.66046511627907"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="10" width="12.6651162790698"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="13.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="13.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="12.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="5" style="10" width="7.66"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="10" width="12.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8825,45 +10295,54 @@
         <v>63</v>
       </c>
     </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="10" t="s">
+        <v>64</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A12" r:id="rId1" display="https://classroom.udacity.com/nanodegrees/nd144/parts/cd0006/modules/859eb994-ce9d-407a-a141-e3efeba6541f/lessons/b7f54535-7631-4b68-a0eb-089e7e2047e2/concepts/8483c9ac-e70f-4f51-8b8f-a6647278f225"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="N18" activeCellId="0" sqref="N18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="12.65625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="14.8325581395349"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="16.8372093023256"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="17.1627906976744"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="8.32558139534884"/>
-    <col collapsed="false" hidden="false" max="24" min="5" style="10" width="7.66046511627907"/>
-    <col collapsed="false" hidden="false" max="1025" min="25" style="10" width="12.6651162790698"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="14.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="16.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="17.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="8.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="5" style="10" width="7.66"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="25" style="10" width="12.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="34" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B1" s="34"/>
       <c r="C1" s="34"/>
@@ -8967,7 +10446,7 @@
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="30" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B12" s="28"/>
       <c r="C12" s="28"/>
@@ -9086,10 +10565,10 @@
         <v>22</v>
       </c>
       <c r="B31" s="41" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C31" s="42" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D31" s="28"/>
     </row>
@@ -9204,7 +10683,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -9213,31 +10692,31 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="12.65625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="13.1581395348837"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="15.1627906976744"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="18.8279069767442"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="10" width="17.8372093023256"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="10" width="17.4976744186047"/>
-    <col collapsed="false" hidden="false" max="26" min="7" style="10" width="7.66046511627907"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="10" width="12.6651162790698"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="13.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="15.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="18.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="10" width="17.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="10" width="17.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="10" width="7.66"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="10" width="12.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="92" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="18" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="18"/>
@@ -9247,10 +10726,10 @@
         <v>22</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9382,7 +10861,7 @@
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="48" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -9391,7 +10870,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>